<commit_message>
Vers 1.1 BMC Gastroenterology
publication version
</commit_message>
<xml_diff>
--- a/input_data/mortality_comparisons.xlsx
+++ b/input_data/mortality_comparisons.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvaughan\Dropbox\WIP\Risk Prediction\RiskEA working\required_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvaughan\Dropbox\WIP\Risk Prediction\GIT\RiskEA working\IC-RISC-Working\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E035E23-062D-4EA1-B688-D4B4A27E9E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="0" windowWidth="22380" windowHeight="11820"/>
+    <workbookView xWindow="16815" yWindow="0" windowWidth="22380" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cum_dis_wide subset" sheetId="2" r:id="rId1"/>
     <sheet name="cum_dis_wide" sheetId="1" r:id="rId2"/>
+    <sheet name="NOTES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="17">
   <si>
     <t>age</t>
   </si>
@@ -69,11 +71,14 @@
   <si>
     <t>Traffic</t>
   </si>
+  <si>
+    <t>The first sheet (subset) is used in the program. It is a subset of the actual data (second sheet), created by zero-ing out risks that overlap (have similar absolute risk) with others. This is purely an arbitray fix for visibility.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,10 +878,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -2409,7 +2414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3932,4 +3937,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D8B4C-DB36-4DF0-AB8D-B382E2B3177B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Vers 1.1 BMC Gastroenterology"
This reverts commit c8be2fe7d71e29e42ea91d2e6f222fe2b1016301.
</commit_message>
<xml_diff>
--- a/input_data/mortality_comparisons.xlsx
+++ b/input_data/mortality_comparisons.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvaughan\Dropbox\WIP\Risk Prediction\GIT\RiskEA working\IC-RISC-Working\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvaughan\Dropbox\WIP\Risk Prediction\RiskEA working\required_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E035E23-062D-4EA1-B688-D4B4A27E9E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16815" yWindow="0" windowWidth="22380" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="0" windowWidth="22380" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="cum_dis_wide subset" sheetId="2" r:id="rId1"/>
     <sheet name="cum_dis_wide" sheetId="1" r:id="rId2"/>
-    <sheet name="NOTES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="16">
   <si>
     <t>age</t>
   </si>
@@ -71,14 +69,11 @@
   <si>
     <t>Traffic</t>
   </si>
-  <si>
-    <t>The first sheet (subset) is used in the program. It is a subset of the actual data (second sheet), created by zero-ing out risks that overlap (have similar absolute risk) with others. This is purely an arbitray fix for visibility.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -878,10 +873,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -2414,7 +2409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3937,22 +3932,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D8B4C-DB36-4DF0-AB8D-B382E2B3177B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Vers 1.1 BMC Gastroenterology""
This reverts commit 12ea4e66603b704d40515c8a842647a64e5cbe11.
</commit_message>
<xml_diff>
--- a/input_data/mortality_comparisons.xlsx
+++ b/input_data/mortality_comparisons.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvaughan\Dropbox\WIP\Risk Prediction\RiskEA working\required_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tvaughan\Dropbox\WIP\Risk Prediction\GIT\RiskEA working\IC-RISC-Working\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E035E23-062D-4EA1-B688-D4B4A27E9E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="0" windowWidth="22380" windowHeight="11820"/>
+    <workbookView xWindow="16815" yWindow="0" windowWidth="22380" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cum_dis_wide subset" sheetId="2" r:id="rId1"/>
     <sheet name="cum_dis_wide" sheetId="1" r:id="rId2"/>
+    <sheet name="NOTES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="17">
   <si>
     <t>age</t>
   </si>
@@ -69,11 +71,14 @@
   <si>
     <t>Traffic</t>
   </si>
+  <si>
+    <t>The first sheet (subset) is used in the program. It is a subset of the actual data (second sheet), created by zero-ing out risks that overlap (have similar absolute risk) with others. This is purely an arbitray fix for visibility.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,10 +878,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -2409,7 +2414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3932,4 +3937,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D8B4C-DB36-4DF0-AB8D-B382E2B3177B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>